<commit_message>
Updated cp and ic
</commit_message>
<xml_diff>
--- a/int_sum.xlsx
+++ b/int_sum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="14895" windowHeight="7875" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="14895" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="CT-IP" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
   <si>
     <t>bk</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>2X0XX1506600</t>
+  </si>
+  <si>
+    <t>0X0XX8501300</t>
+  </si>
+  <si>
+    <t>INT 2013 QT-2</t>
   </si>
 </sst>
 </file>
@@ -526,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -921,31 +927,64 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="J16" s="3">
-        <f>SUM(J3:J14)</f>
-        <v>7562</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="F18" s="8"/>
-      <c r="I18" s="4" t="s">
+    <row r="15" spans="1:10">
+      <c r="A15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="4">
+        <v>30000</v>
+      </c>
+      <c r="C15" s="5">
+        <v>41975</v>
+      </c>
+      <c r="D15" s="4">
+        <v>7.75</v>
+      </c>
+      <c r="E15" s="4">
+        <v>61</v>
+      </c>
+      <c r="F15" s="6">
+        <v>395</v>
+      </c>
+      <c r="G15" s="5">
+        <v>42037</v>
+      </c>
+      <c r="H15" s="8">
+        <v>30395</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="8">
+        <f>H15-B15</f>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="J17" s="3">
+        <f>SUM(J3:J15)</f>
+        <v>7957</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="F19" s="8"/>
+      <c r="I19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J19" s="8">
         <v>299</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B21" s="12">
         <v>41925</v>
       </c>
-      <c r="J20" s="3">
-        <f>J16+J18*2</f>
-        <v>8160</v>
+      <c r="J21" s="3">
+        <f>J17+J19*2</f>
+        <v>8555</v>
       </c>
     </row>
   </sheetData>
@@ -958,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1649,10 +1688,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1725,22 +1764,31 @@
       <c r="B3" s="4">
         <v>50000</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="5">
+        <v>41925</v>
+      </c>
       <c r="D3" s="4">
         <v>9</v>
       </c>
       <c r="E3" s="4">
         <v>390</v>
       </c>
-      <c r="F3" s="4">
-        <v>5000</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4">
-        <f>F3</f>
-        <v>5000</v>
+      <c r="F3" s="8">
+        <f xml:space="preserve"> ( ( (B3*D3/100) / 365 ) * E3 )</f>
+        <v>4808.2191780821913</v>
+      </c>
+      <c r="G3" s="5">
+        <v>42313</v>
+      </c>
+      <c r="H3" s="8">
+        <f>B3+F3</f>
+        <v>54808.219178082189</v>
+      </c>
+      <c r="I3" s="4">
+        <v>4710071983</v>
+      </c>
+      <c r="J3" s="8">
+        <v>2500</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -1749,43 +1797,187 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4">
+        <v>25000</v>
+      </c>
+      <c r="C4" s="5">
+        <v>41947</v>
+      </c>
+      <c r="D4" s="4">
+        <v>7.75</v>
+      </c>
+      <c r="E4" s="4">
+        <v>61</v>
+      </c>
+      <c r="F4" s="8">
+        <f xml:space="preserve"> ( ( (B4*D4/100) / 365 ) * E4 )</f>
+        <v>323.80136986301369</v>
+      </c>
+      <c r="G4" s="5">
+        <v>42009</v>
+      </c>
+      <c r="H4" s="8">
+        <f>B4+F4</f>
+        <v>25323.801369863013</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4710072323</v>
+      </c>
+      <c r="J4" s="8">
+        <f>F4</f>
+        <v>323.80136986301369</v>
+      </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="M4" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="4">
-        <v>744</v>
+      <c r="A5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="4">
+        <v>25000</v>
+      </c>
+      <c r="C5" s="5">
+        <v>41975</v>
+      </c>
+      <c r="D5" s="4">
+        <v>8.75</v>
+      </c>
+      <c r="E5" s="4">
+        <v>390</v>
+      </c>
+      <c r="F5" s="8">
+        <f xml:space="preserve"> ( ( (B5*D5/100) / 365 ) * E5 )</f>
+        <v>2337.3287671232879</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="8">
+        <f>B5+F5</f>
+        <v>27337.328767123287</v>
+      </c>
+      <c r="I5" s="4">
+        <v>4713004066</v>
+      </c>
+      <c r="J5" s="8">
+        <f>F5</f>
+        <v>2337.3287671232879</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="J7" s="1">
-        <f>J3 + J5 * 4</f>
-        <v>7976</v>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="8">
+        <f>J3+J5</f>
+        <v>4837.3287671232883</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="4">
+        <v>744</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="4">
+        <v>372</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="J12" s="4">
+        <f>J9+J10</f>
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="J14" s="1">
+        <f xml:space="preserve"> J7 + J12*2</f>
+        <v>7069.3287671232883</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="5">
+        <v>41975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>